<commit_message>
Update conception projet Web.xlsx
</commit_message>
<xml_diff>
--- a/conception projet Web.xlsx
+++ b/conception projet Web.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rindrarolando/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rindrarolando/IntelliJ/Projet-Cloud-mobile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47D4044-EA7B-D64B-8B05-04A9254B6B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022DA765-D9F4-144E-A32A-D732FD1F2229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{21F81D28-741C-CD42-8B67-26034A88C1AA}"/>
   </bookViews>
@@ -599,7 +599,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA3445D-93A5-BE4C-ABA2-FF437B44F96C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -637,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -657,7 +656,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -697,7 +696,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -717,7 +716,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -757,7 +756,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -777,7 +776,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -817,7 +816,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -837,7 +836,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -877,7 +876,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -897,7 +896,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -937,7 +936,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -957,7 +956,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -997,7 +996,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +1016,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
@@ -1057,7 +1056,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
@@ -1077,7 +1076,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1116,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1176,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1197,7 +1196,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
@@ -1217,7 +1216,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
@@ -1237,7 +1236,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -1257,7 +1256,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
@@ -1277,7 +1276,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1370,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1384,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
@@ -1399,7 +1398,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>37</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>41</v>
       </c>
@@ -1424,7 +1423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>49</v>
       </c>
@@ -1522,7 +1521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>52</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>55</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
@@ -1597,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="C55" t="s">
         <v>59</v>
@@ -1615,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="C56" s="4" t="s">
         <v>58</v>
@@ -1632,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="C57" s="4" t="s">
         <v>59</v>
@@ -1686,13 +1685,7 @@
       <c r="A69" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F57" xr:uid="{6CA3445D-93A5-BE4C-ABA2-FF437B44F96C}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Rindra"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F57" xr:uid="{6CA3445D-93A5-BE4C-ABA2-FF437B44F96C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>